<commit_message>
adding snapshot for api and webservice testing learning
</commit_message>
<xml_diff>
--- a/Study Plan.xlsx
+++ b/Study Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5555B708-EF7F-453D-A6D5-F6B2D50E7851}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF819653-AA43-4624-ADAA-4CAEBEAB38F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{C5A3A7DF-2704-4226-BB77-DE36F17AC19B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{C5A3A7DF-2704-4226-BB77-DE36F17AC19B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Python" sheetId="3" r:id="rId3"/>
     <sheet name="SQL" sheetId="4" r:id="rId4"/>
     <sheet name="REST API" sheetId="5" r:id="rId5"/>
+    <sheet name="Maven" sheetId="6" r:id="rId6"/>
+    <sheet name="JSon" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t xml:space="preserve">In next 3 years I will be phd as I need to become data scientist. </t>
   </si>
@@ -128,13 +130,139 @@
   </si>
   <si>
     <t>REST API</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Application programming interface</t>
+  </si>
+  <si>
+    <t>REST</t>
+  </si>
+  <si>
+    <t>Representational State Transfer</t>
+  </si>
+  <si>
+    <t>1.  Architechtural style of web
+2. A standard and set of guidelines to by which we can structure and create API's
+3. REST API has indentifiable properties</t>
+  </si>
+  <si>
+    <t>Question: what are these properties:???</t>
+  </si>
+  <si>
+    <t>Answers:</t>
+  </si>
+  <si>
+    <t>1. They made use of resource based URLs
+Ex: Webpage: www.football.com/scores- this url is like a get request a qery to web page and it will show results
+Json: www.football.com/api/scores- this is like endpoint which gives json data which we can use in our code
+2. They made use of HTTP methods
+    -GET: To retrieve data from server
+    -POST-To send data to server
+   -PUT: To update data
+   -DELETE: To delete data
+3. They made use of HTTP status code
+     Example: 200 means OK, 404- resourse not found, 500 server error</t>
+  </si>
+  <si>
+    <t>1.  http://maps.google.com/maps/api/geocode/json?address=chicago&amp;sensor=false this a URL of map api , below are it's components
+a. Server: maps.google.com
+b. Resourses: maps, api, geocode,json
+c. parameters: address=chicago</t>
+  </si>
+  <si>
+    <t>Good Site for POSTMAN Test</t>
+  </si>
+  <si>
+    <t>https://reqres.in</t>
+  </si>
+  <si>
+    <t>What Is Swagger?</t>
+  </si>
+  <si>
+    <t>Swagger allows you to describe the structure of your APIs so that machines can read them. The ability of APIs to describe their own structure is the root of all awesomeness in Swagger. Why is it so great? Well, by reading your API’s structure, we can automatically build beautiful and interactive API documentation. We can also automatically generate client libraries for your API in many languages and explore other possibilities like automated testing. Swagger does this by asking your API to return a YAML or JSON that contains a detailed description of your entire API. This file is essentially a resource listing of your API which adheres to OpenAPI Specification. The specification asks you to include information like:
+What are all the operations that your API supports?
+What are your API’s parameters and what does it return?
+Does your API need some authorization?
+And even fun things like terms, contact information and license to use the API.
+You can write a Swagger spec for your API manually, or have it generated automatically from annotations in your source code. Check swagger.io/open-source-integrations for a list of tools that let you generate Swagger from code.</t>
+  </si>
+  <si>
+    <t>http://services.groupkt.com/post/c9b0ccb9/restful-webservices-to-get-and-search-countries.htm</t>
+  </si>
+  <si>
+    <t>Archtype</t>
+  </si>
+  <si>
+    <t>What is Archetype?
+In short, Archetype is a Maven project templating toolkit. An archetype is defined as an original pattern or model from which all other things of the same kind are made. The name fits as we are trying to provide a system that provides a consistent means of generating Maven projects. Archetype will help authors create Maven project templates for users, and provides users with the means to generate parameterized versions of those project templates</t>
+  </si>
+  <si>
+    <t>Marshaling:</t>
+  </si>
+  <si>
+    <t>Unmarshalling:</t>
+  </si>
+  <si>
+    <t>Convert object to json quickly:</t>
+  </si>
+  <si>
+    <t>1. Launch Firefox/Chrome/Safari
+2. Open Firebug/developer tools
+3. Copy/paste your code into the console.
+Then type console.log(JSON.stringify(object)) and voila!
+var object = {
+  item1: 'value1',
+  item2: 1000,
+  item3: ['a', 'b', 'c'],
+  item4: [1, 2, 3],
+  item5: {
+    foo: 'bar'
+  }
+};
+console.log(JSON.stringify(object))
+Output:
+{"item1":"value1","item2":1000,"item3":["a","b","c"],
+ "item4":[1,2,3],"item5":{"foo":"bar"}}
+Copy/paste back into your text editor.</t>
+  </si>
+  <si>
+    <t>POJO</t>
+  </si>
+  <si>
+    <t>plain old java object</t>
+  </si>
+  <si>
+    <t>Convert object(POJO) to json</t>
+  </si>
+  <si>
+    <t>Convert json to object(POJO)</t>
+  </si>
+  <si>
+    <t>eclipse set up project</t>
+  </si>
+  <si>
+    <t>1.create a maven project give a group id and  a artifact id.
+2. delete default package in test and main folder of project
+3. In POM.xml- delete Junit as we don't need it
+4. Add Http client maven dependency(latest version: 4.5.8)
+5. add http core library(latest: 4.4.11)
+6. TESTNG, Json parser maven</t>
+  </si>
+  <si>
+    <t>For Json validation</t>
+  </si>
+  <si>
+    <t>JSONLINT.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +277,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,19 +310,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -716,28 +877,1313 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F0D801-826A-483D-8470-75DCB78FD3A9}">
-  <dimension ref="H1:L1"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B29:O39"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="B10:I14"/>
+    <mergeCell ref="C16:O25"/>
+    <mergeCell ref="B4:P6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" xr:uid="{3EC09E5B-CF97-4537-81C4-B3EF62D27776}"/>
+    <hyperlink ref="D28" r:id="rId2" xr:uid="{C86F6791-9150-4E66-8240-320AFB02E1EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7382F2FE-111D-40F1-8C38-CA377BEA7268}">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="8:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="H1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="A2:T16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89548132-52F6-4374-9047-A9E11A0FEC3D}">
+  <dimension ref="A1:N34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B5:K20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>